<commit_message>
Update Optimal storage dispatch scenarios.xlsx
Update the parameter descriptions
</commit_message>
<xml_diff>
--- a/Optimal storage dispatch scenarios.xlsx
+++ b/Optimal storage dispatch scenarios.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Total capacity</t>
   </si>
@@ -43,70 +43,58 @@
     <t>/month</t>
   </si>
   <si>
-    <t>Daily cycle cost</t>
-  </si>
-  <si>
-    <t>/day</t>
-  </si>
-  <si>
-    <t>Hourly cost</t>
-  </si>
-  <si>
-    <t>/hour</t>
-  </si>
-  <si>
-    <t>Ps_base</t>
+    <t>Base case storage price</t>
   </si>
   <si>
     <t>/MWh.h</t>
   </si>
   <si>
-    <t>Reservation</t>
+    <t>Reservation storage capacity</t>
   </si>
   <si>
     <t>of total</t>
   </si>
   <si>
-    <t>Ps_study</t>
-  </si>
-  <si>
-    <t>Pp</t>
+    <t>Study case storage price</t>
+  </si>
+  <si>
+    <t>Energy Price</t>
   </si>
   <si>
     <t>/MWh</t>
   </si>
   <si>
-    <t>Qs</t>
-  </si>
-  <si>
-    <t>Qp</t>
+    <t>Storage capacity</t>
+  </si>
+  <si>
+    <t>Power capacity</t>
   </si>
   <si>
     <t>MW</t>
   </si>
   <si>
-    <t>Cs_base</t>
-  </si>
-  <si>
-    <t>$/h</t>
-  </si>
-  <si>
-    <t>Cs_study</t>
-  </si>
-  <si>
-    <t>Cp</t>
-  </si>
-  <si>
-    <t>a (base case)</t>
+    <t>Base case hourly storage cost</t>
+  </si>
+  <si>
+    <t>/h</t>
+  </si>
+  <si>
+    <t>Study case hourly storage cost</t>
+  </si>
+  <si>
+    <t>Hourly energy cost</t>
+  </si>
+  <si>
+    <t>Base case storage price sensitivity (a)</t>
   </si>
   <si>
     <t>/MW^2.h^3</t>
   </si>
   <si>
-    <t>a (study case)</t>
-  </si>
-  <si>
-    <t>c (both cases)</t>
+    <t>Study case storage price sensitivity (a)</t>
+  </si>
+  <si>
+    <t>Energy price sensitivity (c)</t>
   </si>
   <si>
     <t>/MW^2.h</t>
@@ -382,7 +370,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.88"/>
+    <col customWidth="1" min="1" max="1" width="29.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -452,8 +440,8 @@
         <v>10</v>
       </c>
       <c r="B7" s="5">
-        <f>B6/30</f>
-        <v>404.4253145</v>
+        <f>B6/B1</f>
+        <v>12.13275944</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
@@ -463,9 +451,8 @@
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5">
-        <f>B7/12</f>
-        <v>33.70210954</v>
+      <c r="B8" s="4">
+        <v>0.2</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -476,89 +463,90 @@
         <v>14</v>
       </c>
       <c r="B9" s="5">
-        <f>B6/B1</f>
-        <v>12.13275944</v>
+        <f>B7*B8</f>
+        <v>2.426551887</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3">
+        <v>100.0</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5">
-        <f>B9*B10</f>
-        <v>2.426551887</v>
+        <v>17</v>
+      </c>
+      <c r="B11" s="6">
+        <f>B12*0.15</f>
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" s="3">
-        <v>100.0</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5">
+        <f>B11*B7</f>
+        <v>181.9913915</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B13" s="6">
-        <f>B14*0.15</f>
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="1">
-        <v>100.0</v>
+      <c r="B14" s="5">
+        <f t="shared" ref="B14:B15" si="1">B11*B9</f>
+        <v>36.39827831</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="5">
-        <f>B13*B9</f>
-        <v>181.9913915</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="7">
+        <f t="shared" si="1"/>
+        <v>10000</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5">
-        <f t="shared" ref="B16:B17" si="1">B13*B11</f>
-        <v>36.39827831</v>
+        <f>2*B13/B11^2</f>
+        <v>1.617701258</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
@@ -566,11 +554,11 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="7">
-        <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>26</v>
+      </c>
+      <c r="B17" s="5">
+        <f t="shared" ref="B17:B18" si="2">2*B14/B11^2</f>
+        <v>0.3235402516</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
@@ -578,38 +566,14 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="5">
-        <f>2*B15/B13^2</f>
-        <v>1.617701258</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="5">
-        <f t="shared" ref="B19:B20" si="2">2*B16/B13^2</f>
-        <v>0.3235402516</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="7">
+        <v>27</v>
+      </c>
+      <c r="B18" s="7">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>32</v>
+      <c r="C18" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>